<commit_message>
last commit did not get packaged...
</commit_message>
<xml_diff>
--- a/gnosis_cheatsheet.xlsx
+++ b/gnosis_cheatsheet.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Storage\Tresorit\Devel\CurseForge\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20316" windowHeight="12816" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20320" windowHeight="12820" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="1" r:id="rId1"/>
@@ -1259,17 +1254,17 @@
       <selection activeCell="F26" sqref="F26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="34.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="34.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="18.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="22.77734375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.81640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.5546875" customWidth="1"/>
-    <col min="6" max="6" width="60.5546875" customWidth="1"/>
+    <col min="5" max="5" width="80.54296875" customWidth="1"/>
+    <col min="6" max="6" width="60.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>140</v>
       </c>
@@ -1300,7 +1295,7 @@
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
     </row>
-    <row r="2" spans="1:17" ht="59.7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>189</v>
       </c>
@@ -1331,7 +1326,7 @@
       <c r="P2" s="2"/>
       <c r="Q2" s="2"/>
     </row>
-    <row r="3" spans="1:17" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -1360,7 +1355,7 @@
       <c r="P3" s="2"/>
       <c r="Q3" s="2"/>
     </row>
-    <row r="4" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>1</v>
       </c>
@@ -1389,7 +1384,7 @@
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
     </row>
-    <row r="5" spans="1:17" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>28</v>
       </c>
@@ -1418,7 +1413,7 @@
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
     </row>
-    <row r="6" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>51</v>
       </c>
@@ -1447,7 +1442,7 @@
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
     </row>
-    <row r="7" spans="1:17" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="12" t="s">
         <v>3</v>
       </c>
@@ -1476,7 +1471,7 @@
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
     </row>
-    <row r="8" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A8" s="12" t="s">
         <v>4</v>
       </c>
@@ -1503,7 +1498,7 @@
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
     </row>
-    <row r="9" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>19</v>
       </c>
@@ -1532,7 +1527,7 @@
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
     </row>
-    <row r="10" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>14</v>
       </c>
@@ -1561,7 +1556,7 @@
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
     </row>
-    <row r="11" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>15</v>
       </c>
@@ -1590,7 +1585,7 @@
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
     </row>
-    <row r="12" spans="1:17" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
@@ -1619,7 +1614,7 @@
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
     </row>
-    <row r="13" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>30</v>
       </c>
@@ -1648,7 +1643,7 @@
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
     </row>
-    <row r="14" spans="1:17" ht="59.7" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:17" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>175</v>
       </c>
@@ -1679,7 +1674,7 @@
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
     </row>
-    <row r="15" spans="1:17" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>7</v>
       </c>
@@ -1710,7 +1705,7 @@
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
     </row>
-    <row r="16" spans="1:17" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>141</v>
       </c>
@@ -1739,7 +1734,7 @@
       <c r="P16" s="2"/>
       <c r="Q16" s="2"/>
     </row>
-    <row r="17" spans="1:17" ht="44.85" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:17" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
@@ -1768,7 +1763,7 @@
       <c r="P17" s="2"/>
       <c r="Q17" s="2"/>
     </row>
-    <row r="18" spans="1:17" ht="59.7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>181</v>
       </c>
@@ -1797,7 +1792,7 @@
       <c r="P18" s="2"/>
       <c r="Q18" s="2"/>
     </row>
-    <row r="19" spans="1:17" ht="238.65" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:17" ht="246.5" x14ac:dyDescent="0.35">
       <c r="A19" s="4" t="s">
         <v>10</v>
       </c>
@@ -1826,7 +1821,7 @@
       <c r="P19" s="2"/>
       <c r="Q19" s="2"/>
     </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
         <v>142</v>
       </c>
@@ -1844,7 +1839,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:17" ht="58" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
         <v>81</v>
       </c>
@@ -1860,7 +1855,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
         <v>18</v>
       </c>
@@ -1878,7 +1873,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
         <v>29</v>
       </c>
@@ -1896,7 +1891,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
         <v>2</v>
       </c>
@@ -1914,7 +1909,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
         <v>16</v>
       </c>
@@ -1932,109 +1927,109 @@
         <v>196</v>
       </c>
     </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A26" s="4"/>
     </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A27" s="4"/>
     </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
     </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A29" s="2"/>
     </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A30" s="4"/>
     </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A31" s="4"/>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A32" s="4"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="4"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="4"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="4"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="4"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="4"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="4"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="4"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="4"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="4"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="4"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="4"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="4"/>
     </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B57" s="1"/>
     </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B58" s="1"/>
     </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B59" s="1"/>
     </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B60" s="1"/>
     </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B61" s="1"/>
     </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B62" s="1"/>
     </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B63" s="1"/>
     </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B64" s="1"/>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B65" s="1"/>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B66" s="1"/>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B67" s="1"/>
     </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B68" s="1"/>
     </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B69" s="1"/>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B70" s="1"/>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B71" s="1"/>
     </row>
   </sheetData>
@@ -2061,16 +2056,16 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="70.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="70.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.77734375" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.81640625" style="7" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="32" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="73.44140625" style="7" customWidth="1"/>
-    <col min="4" max="4" width="49.5546875" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="70.44140625" style="7"/>
+    <col min="3" max="3" width="73.453125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="49.54296875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="70.453125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="10" t="s">
         <v>27</v>
       </c>
@@ -2086,7 +2081,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>199</v>
       </c>
@@ -2102,7 +2097,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="5" t="s">
         <v>137</v>
       </c>
@@ -2118,7 +2113,7 @@
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>184</v>
       </c>
@@ -2134,7 +2129,7 @@
       <c r="E4" s="5"/>
       <c r="F4" s="5"/>
     </row>
-    <row r="5" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>61</v>
       </c>
@@ -2148,7 +2143,7 @@
       <c r="E5" s="5"/>
       <c r="F5" s="5"/>
     </row>
-    <row r="6" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" s="11" t="s">
         <v>79</v>
       </c>
@@ -2164,7 +2159,7 @@
       <c r="E6" s="5"/>
       <c r="F6" s="5"/>
     </row>
-    <row r="7" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" s="11" t="s">
         <v>57</v>
       </c>
@@ -2180,7 +2175,7 @@
       <c r="E7" s="5"/>
       <c r="F7" s="5"/>
     </row>
-    <row r="8" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>60</v>
       </c>
@@ -2194,7 +2189,7 @@
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
     </row>
-    <row r="9" spans="1:6" ht="44.85" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>96</v>
       </c>
@@ -2210,7 +2205,7 @@
       <c r="E9" s="5"/>
       <c r="F9" s="5"/>
     </row>
-    <row r="10" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" s="10" t="s">
         <v>55</v>
       </c>
@@ -2226,7 +2221,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>176</v>
       </c>
@@ -2242,7 +2237,7 @@
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
     </row>
-    <row r="12" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="5" t="s">
         <v>125</v>
       </c>
@@ -2258,7 +2253,7 @@
       <c r="E12" s="5"/>
       <c r="F12" s="5"/>
     </row>
-    <row r="13" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" s="11" t="s">
         <v>177</v>
       </c>
@@ -2272,7 +2267,7 @@
       <c r="E13" s="5"/>
       <c r="F13" s="5"/>
     </row>
-    <row r="14" spans="1:6" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>62</v>
       </c>
@@ -2288,7 +2283,7 @@
       <c r="E14" s="5"/>
       <c r="F14" s="5"/>
     </row>
-    <row r="15" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>94</v>
       </c>
@@ -2302,7 +2297,7 @@
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
     </row>
-    <row r="16" spans="1:6" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>92</v>
       </c>
@@ -2318,7 +2313,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
     </row>
-    <row r="17" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" s="11" t="s">
         <v>90</v>
       </c>
@@ -2332,7 +2327,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
     </row>
-    <row r="18" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>76</v>
       </c>
@@ -2348,7 +2343,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
     </row>
-    <row r="19" spans="1:6" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>80</v>
       </c>
@@ -2364,7 +2359,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
     </row>
-    <row r="20" spans="1:6" ht="59.7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A20" s="5" t="s">
         <v>159</v>
       </c>
@@ -2380,7 +2375,7 @@
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
     </row>
-    <row r="21" spans="1:6" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>89</v>
       </c>
@@ -2396,7 +2391,7 @@
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
     </row>
-    <row r="22" spans="1:6" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>78</v>
       </c>
@@ -2410,7 +2405,7 @@
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" s="11" t="s">
         <v>87</v>
       </c>
@@ -2426,7 +2421,7 @@
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
     </row>
-    <row r="24" spans="1:6" ht="29.85" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>98</v>
       </c>
@@ -2442,7 +2437,7 @@
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
     </row>
-    <row r="25" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="A25" s="5" t="s">
         <v>165</v>
       </c>
@@ -2456,7 +2451,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>83</v>
       </c>
@@ -2468,7 +2463,7 @@
       </c>
       <c r="D26" s="11"/>
     </row>
-    <row r="27" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>99</v>
       </c>
@@ -2482,7 +2477,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" s="11" t="s">
         <v>56</v>
       </c>
@@ -2496,7 +2491,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" s="10" t="s">
         <v>54</v>
       </c>
@@ -2510,7 +2505,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>86</v>
       </c>

</xml_diff>